<commit_message>
parrele exectuion changes, new test in users page
</commit_message>
<xml_diff>
--- a/TestCases/eSealTestCases.xlsx
+++ b/TestCases/eSealTestCases.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="378">
   <si>
     <t xml:space="preserve">SNo</t>
   </si>
@@ -646,6 +646,9 @@
     <t xml:space="preserve">Smoke, Regression</t>
   </si>
   <si>
+    <t xml:space="preserve">Close</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC_002</t>
   </si>
   <si>
@@ -701,6 +704,9 @@
   </si>
   <si>
     <t xml:space="preserve">Verify that the Save and Close button texts are correct.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC006</t>
   </si>
   <si>
     <t xml:space="preserve">TC_010</t>
@@ -2800,10 +2806,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2835,6 +2841,9 @@
       <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
@@ -2855,10 +2864,13 @@
       <c r="F2" s="9" t="s">
         <v>190</v>
       </c>
+      <c r="G2" s="7" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>187</v>
@@ -2867,10 +2879,10 @@
         <v>36</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>16</v>
@@ -2878,7 +2890,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>187</v>
@@ -2887,10 +2899,10 @@
         <v>38</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>16</v>
@@ -2898,7 +2910,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>187</v>
@@ -2907,10 +2919,10 @@
         <v>41</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>16</v>
@@ -2918,7 +2930,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>44</v>
@@ -2927,18 +2939,18 @@
         <v>45</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>44</v>
@@ -2947,10 +2959,10 @@
         <v>47</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>16</v>
@@ -2958,7 +2970,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>44</v>
@@ -2967,10 +2979,10 @@
         <v>49</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>16</v>
@@ -2978,7 +2990,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>44</v>
@@ -2987,10 +2999,10 @@
         <v>51</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>16</v>
@@ -2998,7 +3010,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>44</v>
@@ -3007,18 +3019,21 @@
         <v>53</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>16</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>44</v>
@@ -3027,18 +3042,18 @@
         <v>55</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>44</v>
@@ -3047,10 +3062,10 @@
         <v>58</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>16</v>
@@ -3058,7 +3073,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>44</v>
@@ -3067,18 +3082,18 @@
         <v>61</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>44</v>
@@ -3087,7 +3102,7 @@
         <v>60</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>189</v>
@@ -3098,7 +3113,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>44</v>
@@ -3107,7 +3122,7 @@
         <v>65</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>189</v>
@@ -3118,7 +3133,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>44</v>
@@ -3127,7 +3142,7 @@
         <v>67</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>189</v>
@@ -3138,7 +3153,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>44</v>
@@ -3147,18 +3162,18 @@
         <v>69</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>44</v>
@@ -3167,18 +3182,18 @@
         <v>71</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>44</v>
@@ -3187,10 +3202,10 @@
         <v>73</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>16</v>
@@ -3198,7 +3213,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>44</v>
@@ -3207,10 +3222,10 @@
         <v>75</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>16</v>
@@ -3218,7 +3233,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>44</v>
@@ -3227,10 +3242,10 @@
         <v>77</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>16</v>
@@ -3238,7 +3253,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>44</v>
@@ -3247,10 +3262,10 @@
         <v>79</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>16</v>
@@ -3258,7 +3273,7 @@
     </row>
     <row r="23" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>44</v>
@@ -3267,10 +3282,10 @@
         <v>81</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>16</v>
@@ -3278,7 +3293,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>44</v>
@@ -3287,10 +3302,10 @@
         <v>82</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>16</v>
@@ -3298,7 +3313,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>44</v>
@@ -3307,10 +3322,10 @@
         <v>83</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>16</v>
@@ -3318,7 +3333,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>44</v>
@@ -3327,10 +3342,10 @@
         <v>84</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>16</v>
@@ -3338,16 +3353,16 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>189</v>
@@ -3358,39 +3373,39 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>246</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>244</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>87</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>89</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>16</v>
@@ -3398,19 +3413,19 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>16</v>
@@ -3418,59 +3433,59 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>93</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>95</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>97</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F33" s="9" t="s">
         <v>16</v>
@@ -3478,36 +3493,36 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>98</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>100</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E35" s="9" t="s">
         <v>189</v>
@@ -3518,59 +3533,59 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>102</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="E36" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>104</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E37" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>106</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>16</v>
@@ -3578,19 +3593,19 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F39" s="9" t="s">
         <v>16</v>
@@ -3598,19 +3613,19 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>110</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F40" s="9" t="s">
         <v>16</v>
@@ -3618,19 +3633,19 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>112</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>16</v>
@@ -3638,27 +3653,27 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>114</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="E42" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>116</v>
@@ -3667,7 +3682,7 @@
         <v>117</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="E43" s="9" t="s">
         <v>189</v>
@@ -3678,7 +3693,7 @@
     </row>
     <row r="44" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>116</v>
@@ -3687,18 +3702,18 @@
         <v>118</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="E44" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>116</v>
@@ -3707,10 +3722,10 @@
         <v>120</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F45" s="9" t="s">
         <v>16</v>
@@ -3718,7 +3733,7 @@
     </row>
     <row r="46" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B46" s="9" t="s">
         <v>116</v>
@@ -3727,10 +3742,10 @@
         <v>121</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F46" s="9" t="s">
         <v>16</v>
@@ -3738,19 +3753,19 @@
     </row>
     <row r="47" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>116</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F47" s="9" t="s">
         <v>16</v>
@@ -3758,19 +3773,19 @@
     </row>
     <row r="48" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>116</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F48" s="9" t="s">
         <v>16</v>
@@ -3778,47 +3793,47 @@
     </row>
     <row r="49" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B49" s="9" t="s">
         <v>116</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E49" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>116</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E50" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>116</v>
@@ -3827,18 +3842,18 @@
         <v>130</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="E51" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B52" s="9" t="s">
         <v>116</v>
@@ -3847,7 +3862,7 @@
         <v>132</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E52" s="9" t="s">
         <v>189</v>
@@ -3858,27 +3873,27 @@
     </row>
     <row r="53" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>116</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="E53" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>116</v>
@@ -3887,30 +3902,30 @@
         <v>135</v>
       </c>
       <c r="D54" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="F54" s="9" t="s">
         <v>306</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="F54" s="9" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>116</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F55" s="9" t="s">
         <v>16</v>
@@ -3918,7 +3933,7 @@
     </row>
     <row r="56" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="9" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>116</v>
@@ -3927,18 +3942,18 @@
         <v>139</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="E56" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="9" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B57" s="9" t="s">
         <v>141</v>
@@ -3947,7 +3962,7 @@
         <v>142</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="E57" s="9" t="s">
         <v>189</v>
@@ -3958,7 +3973,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="9" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>141</v>
@@ -3967,7 +3982,7 @@
         <v>144</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E58" s="9" t="s">
         <v>189</v>
@@ -3978,7 +3993,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="9" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B59" s="9" t="s">
         <v>141</v>
@@ -3987,7 +4002,7 @@
         <v>146</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E59" s="9" t="s">
         <v>189</v>
@@ -3998,7 +4013,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="9" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>141</v>
@@ -4007,38 +4022,38 @@
         <v>148</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E60" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="9" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>141</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="9" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B62" s="9" t="s">
         <v>141</v>
@@ -4047,18 +4062,18 @@
         <v>152</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="9" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B63" s="9" t="s">
         <v>141</v>
@@ -4067,67 +4082,67 @@
         <v>154</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="E63" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="9" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B64" s="9" t="s">
         <v>141</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B65" s="9" t="s">
         <v>141</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E65" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C66" s="9" t="s">
         <v>161</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E66" s="9" t="s">
         <v>189</v>
@@ -4138,16 +4153,16 @@
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="B67" s="9" t="s">
         <v>338</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>336</v>
       </c>
       <c r="C67" s="9" t="s">
         <v>162</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E67" s="9" t="s">
         <v>189</v>
@@ -4158,16 +4173,16 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="9" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C68" s="9" t="s">
         <v>163</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="E68" s="9" t="s">
         <v>189</v>
@@ -4178,36 +4193,36 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="9" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C69" s="9" t="s">
         <v>164</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="E69" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="9" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C70" s="9" t="s">
         <v>165</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="E70" s="9" t="s">
         <v>189</v>
@@ -4218,16 +4233,16 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="9" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C71" s="9" t="s">
         <v>166</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="E71" s="9" t="s">
         <v>189</v>
@@ -4238,19 +4253,19 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="9" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C72" s="9" t="s">
         <v>167</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F72" s="9" t="s">
         <v>16</v>
@@ -4258,19 +4273,19 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="9" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C73" s="9" t="s">
         <v>168</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F73" s="9" t="s">
         <v>16</v>
@@ -4278,39 +4293,39 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="9" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C74" s="9" t="s">
         <v>169</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="9" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C75" s="9" t="s">
         <v>170</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F75" s="9" t="s">
         <v>16</v>
@@ -4318,16 +4333,16 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="9" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C76" s="9" t="s">
         <v>172</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="E76" s="9" t="s">
         <v>189</v>
@@ -4338,16 +4353,16 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="B77" s="9" t="s">
         <v>359</v>
-      </c>
-      <c r="B77" s="9" t="s">
-        <v>357</v>
       </c>
       <c r="C77" s="9" t="s">
         <v>173</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="E77" s="9" t="s">
         <v>189</v>
@@ -4358,16 +4373,16 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="9" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C78" s="9" t="s">
         <v>174</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="E78" s="9" t="s">
         <v>189</v>
@@ -4378,16 +4393,16 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="9" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C79" s="9" t="s">
         <v>175</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="E79" s="9" t="s">
         <v>189</v>
@@ -4398,16 +4413,16 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="9" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C80" s="9" t="s">
         <v>176</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="E80" s="9" t="s">
         <v>189</v>
@@ -4418,59 +4433,59 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="9" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C81" s="9" t="s">
         <v>177</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="E81" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F81" s="9" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="9" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C82" s="9" t="s">
         <v>178</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="E82" s="9" t="s">
         <v>189</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="9" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C83" s="9" t="s">
         <v>179</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F83" s="9" t="s">
         <v>16</v>
@@ -4478,22 +4493,22 @@
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="9" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C84" s="9" t="s">
         <v>180</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>